<commit_message>
Idaho Water Allocation Readme
Idaho Water Allocation Readme
</commit_message>
<xml_diff>
--- a/Idaho/WaterAllocation/ID_Allocation Schema Mapping to WaDE_QA.xlsx
+++ b/Idaho/WaterAllocation/ID_Allocation Schema Mapping to WaDE_QA.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rjame\Documents\WSWC Documents\MappingStatesDataToWaDE2.0\Idaho\WaterAllocation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4517C5FF-A9B9-4519-ACC0-8B885D561C2A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF14B78C-B5AE-4295-B477-5A34B4A59E9A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38520" yWindow="-2550" windowWidth="38640" windowHeight="21240" tabRatio="714" xr2:uid="{10FC1BAB-5472-410C-A2F0-85DCDF5389F8}"/>
+    <workbookView xWindow="-23148" yWindow="1692" windowWidth="23256" windowHeight="12576" tabRatio="714" activeTab="4" xr2:uid="{10FC1BAB-5472-410C-A2F0-85DCDF5389F8}"/>
   </bookViews>
   <sheets>
     <sheet name="Mapping Notes" sheetId="10" r:id="rId1"/>
@@ -2504,7 +2504,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7154D4B-C952-456C-B506-1C3DB2041E3D}">
   <dimension ref="A1:B26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
@@ -3719,8 +3719,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DC5F405-0A84-4CAE-BAB0-9DF044EAE9B9}">
   <dimension ref="A1:J13"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="M10" sqref="M10"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4022,8 +4022,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10E7F0DF-14BE-4BB8-BB6C-8815808B0B66}">
   <dimension ref="A1:J22"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView topLeftCell="A4" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>